<commit_message>
working on big chart
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Old house</t>
   </si>
@@ -47,6 +47,27 @@
   </si>
   <si>
     <t xml:space="preserve">Grain Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total of all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total of appartments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total of houses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total of land</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Land % in portfolio:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Houses % in portfolio:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apartments % in portfolio:</t>
   </si>
 </sst>
 </file>
@@ -56,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -78,6 +99,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,8 +149,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -144,16 +175,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -381,6 +414,83 @@
       </c>
       <c r="G10" s="0" t="n">
         <v>47000</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>6275000</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>6728000</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>7354000</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>7435500</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>7468000</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>8083000</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <f aca="false">SUM(G4,G5)</f>
+        <v>3778000</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">SUM(G2,G6,G7,G8,G9)</f>
+        <v>4195000</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">SUM(G3,G10)</f>
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">SUM(B14*100/G11)</f>
+        <v>1.36088086106644</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <f aca="false">SUM(B13*100/G11)</f>
+        <v>51.8990473833973</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <f aca="false">SUM(B12*100/G11)</f>
+        <v>46.7400717555363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on big chart, trying to make it change shape
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t xml:space="preserve">Old house</t>
   </si>
@@ -49,25 +51,16 @@
     <t xml:space="preserve">Grain Field</t>
   </si>
   <si>
-    <t xml:space="preserve">Total of all</t>
+    <t xml:space="preserve">Total of land</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total of all:</t>
   </si>
   <si>
     <t xml:space="preserve">Total of appartments</t>
   </si>
   <si>
     <t xml:space="preserve">Total of houses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total of land</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Land % in portfolio:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Houses % in portfolio:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apartments % in portfolio:</t>
   </si>
 </sst>
 </file>
@@ -149,8 +142,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -175,10 +172,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -417,80 +414,35 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>6275000</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>6728000</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>7354000</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>7435500</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>7468000</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>8083000</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <f aca="false">SUM(G4,G5)</f>
-        <v>3778000</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <f aca="false">SUM(G2,G6,G7,G8,G9)</f>
-        <v>4195000</v>
-      </c>
+      <c r="C11" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" s="0" t="n">
+        <f aca="false">SUM(B3,B10)</f>
+        <v>81000</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <f aca="false">SUM(C3,C10)</f>
+        <v>79000</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">SUM(D3,D10)</f>
+        <v>79000</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">SUM(E3,E10)</f>
+        <v>89000</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <f aca="false">SUM(F3,F10)</f>
+        <v>87000</v>
+      </c>
+      <c r="G14" s="0" t="n">
         <f aca="false">SUM(G3,G10)</f>
         <v>110000</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <f aca="false">SUM(B14*100/G11)</f>
-        <v>1.36088086106644</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <f aca="false">SUM(B13*100/G11)</f>
-        <v>51.8990473833973</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <f aca="false">SUM(B12*100/G11)</f>
-        <v>46.7400717555363</v>
       </c>
     </row>
   </sheetData>
@@ -502,4 +454,193 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.36"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="n">
+        <v>1995</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>2005</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>2010</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>6275000</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>6728000</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>7354000</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>7435500</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>7468000</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>8083000</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.36"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="n">
+        <v>1995</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>2005</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>2010</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>3254000</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3458000</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>3512000</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>3198000</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>3344000</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>3778000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2940000</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>3191000</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>3763000</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>4148500</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>4037000</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>4195000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>81000</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>79000</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>79000</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>89000</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>87000</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>110000</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finally fixed big Chart problem with .destroy function
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Total of all:</t>
   </si>
   <si>
-    <t xml:space="preserve">Total of appartments</t>
+    <t xml:space="preserve">Total of apartments</t>
   </si>
   <si>
     <t xml:space="preserve">Total of houses</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Total of land</t>
   </si>
   <si>
-    <t xml:space="preserve">Total of appartments </t>
+    <t xml:space="preserve">Total of apartments </t>
   </si>
   <si>
     <t xml:space="preserve">51,899047383</t>
@@ -86,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -108,12 +108,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,16 +152,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -191,7 +181,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -447,8 +437,8 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -520,7 +510,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -636,13 +626,13 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.36"/>
   </cols>
@@ -669,7 +659,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="0" t="s">

</xml_diff>

<commit_message>
Fixed and stylized charts
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t xml:space="preserve">Old house</t>
   </si>
@@ -64,19 +64,25 @@
     <t xml:space="preserve">Total of land</t>
   </si>
   <si>
+    <t xml:space="preserve">Property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent</t>
+  </si>
+  <si>
     <t xml:space="preserve">Total of apartments </t>
   </si>
   <si>
-    <t xml:space="preserve">51,899047383</t>
+    <t xml:space="preserve">51,89</t>
   </si>
   <si>
     <t xml:space="preserve">Total of houses </t>
   </si>
   <si>
-    <t xml:space="preserve">46,740071756</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,360880861</t>
+    <t xml:space="preserve">46,74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,36</t>
   </si>
 </sst>
 </file>
@@ -437,8 +443,8 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -626,8 +632,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -638,24 +644,27 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="n">
-        <v>2020</v>
+      <c r="A1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,7 +672,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>